<commit_message>
aldo:changes in template checklist
</commit_message>
<xml_diff>
--- a/public/templates/Plantilla Checklist.xlsx
+++ b/public/templates/Plantilla Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\gestor\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB8B88A-00EB-43A7-8C24-B4564D571DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA21D5A5-110E-4B8C-8103-E421C3A72953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla Checklist" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Actividad</t>
   </si>
@@ -124,12 +124,36 @@
       <t>(Sí/No)</t>
     </r>
   </si>
+  <si>
+    <t>Actividad 1</t>
+  </si>
+  <si>
+    <t>Opción única</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Actividad 2</t>
+  </si>
+  <si>
+    <t>Escala de evaluación</t>
+  </si>
+  <si>
+    <t>Actividad 3</t>
+  </si>
+  <si>
+    <t>Actividad 4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -149,6 +173,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -228,6 +260,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,22 +606,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
     <col min="3" max="3" width="24.5" customWidth="1"/>
-    <col min="4" max="4" width="37.25" customWidth="1"/>
-    <col min="5" max="5" width="32.875" customWidth="1"/>
+    <col min="4" max="4" width="37.19921875" customWidth="1"/>
+    <col min="5" max="5" width="32.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -604,7 +638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -620,6 +654,77 @@
       <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>